<commit_message>
validamos el flujo de registro, registroEspecial y ambas etiquetas
</commit_message>
<xml_diff>
--- a/docs/junio24/GAFETES POR EXPOSITOR.xlsx
+++ b/docs/junio24/GAFETES POR EXPOSITOR.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yellowhat\proyectos\comexane\docs\junio24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E21680-B112-4458-9668-DEC3D36A72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72097476-0AAC-4559-BF33-C6AF59EACAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A9200D66-FB7D-4255-930C-9F7C00E64FDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A9200D66-FB7D-4255-930C-9F7C00E64FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Mysql" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$3:$E$51</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -229,6 +230,36 @@
   </si>
   <si>
     <t>MINDRAY MÉXICO</t>
+  </si>
+  <si>
+    <t>ASOKAM</t>
+  </si>
+  <si>
+    <t>EVENT MAKERS</t>
+  </si>
+  <si>
+    <t>idExpositor</t>
+  </si>
+  <si>
+    <t>numStandExpositor</t>
+  </si>
+  <si>
+    <t>empresaExpositor</t>
+  </si>
+  <si>
+    <t>numMaximoGafetes</t>
+  </si>
+  <si>
+    <t>numGafetesImpresos</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>modifiedAt</t>
+  </si>
+  <si>
+    <t>esActivo</t>
   </si>
 </sst>
 </file>
@@ -236,7 +267,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -489,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -498,15 +529,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,8 +874,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:L51"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.25"/>
@@ -899,7 +928,6 @@
       <c r="E4" s="5">
         <v>6</v>
       </c>
-      <c r="F4" s="26"/>
       <c r="G4" s="21">
         <f>A4</f>
         <v>101</v>
@@ -937,7 +965,6 @@
       <c r="E5" s="8">
         <v>12</v>
       </c>
-      <c r="F5" s="26"/>
       <c r="G5" s="21">
         <f t="shared" ref="G5:G8" si="0">A5</f>
         <v>102</v>
@@ -976,7 +1003,6 @@
       <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="26"/>
       <c r="G6" s="21">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -1015,7 +1041,6 @@
       <c r="E7" s="10">
         <v>6</v>
       </c>
-      <c r="F7" s="26"/>
       <c r="G7" s="21">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -1053,7 +1078,6 @@
       <c r="E8" s="8">
         <v>12</v>
       </c>
-      <c r="F8" s="26"/>
       <c r="G8" s="21">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -1090,7 +1114,7 @@
       <c r="E9" s="10">
         <v>3</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="26"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -1114,7 +1138,6 @@
       <c r="E10" s="10">
         <v>3</v>
       </c>
-      <c r="F10" s="26"/>
       <c r="G10" s="21">
         <f t="shared" ref="G10:G11" si="2">A10</f>
         <v>113</v>
@@ -1153,7 +1176,6 @@
       <c r="E11" s="8">
         <v>6</v>
       </c>
-      <c r="F11" s="26"/>
       <c r="G11" s="21">
         <f t="shared" si="2"/>
         <v>114</v>
@@ -1190,7 +1212,6 @@
       <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="26"/>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
@@ -1214,7 +1235,6 @@
       <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F13" s="26"/>
       <c r="G13" s="21">
         <f t="shared" ref="G13:G16" si="5">A13</f>
         <v>116</v>
@@ -1253,7 +1273,6 @@
       <c r="E14" s="8">
         <v>3</v>
       </c>
-      <c r="F14" s="26"/>
       <c r="G14" s="21">
         <f t="shared" si="5"/>
         <v>117</v>
@@ -1290,7 +1309,6 @@
       <c r="E15" s="16">
         <v>2</v>
       </c>
-      <c r="F15" s="26"/>
       <c r="G15" s="21">
         <f t="shared" si="5"/>
         <v>119</v>
@@ -1329,7 +1347,6 @@
       <c r="E16" s="8">
         <v>6</v>
       </c>
-      <c r="F16" s="26"/>
       <c r="G16" s="21">
         <f t="shared" si="5"/>
         <v>120</v>
@@ -1364,7 +1381,6 @@
       <c r="E17" s="8">
         <v>2</v>
       </c>
-      <c r="F17" s="26"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
@@ -1384,7 +1400,6 @@
       <c r="E18" s="8">
         <v>2</v>
       </c>
-      <c r="F18" s="26"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
@@ -1406,7 +1421,6 @@
       <c r="E19" s="8">
         <v>2</v>
       </c>
-      <c r="F19" s="26"/>
       <c r="G19" s="21">
         <f t="shared" ref="G19:G51" si="8">A19</f>
         <v>124</v>
@@ -1443,7 +1457,6 @@
       <c r="E20" s="8">
         <v>2</v>
       </c>
-      <c r="F20" s="26"/>
       <c r="G20" s="21">
         <f t="shared" si="8"/>
         <v>125</v>
@@ -1482,14 +1495,12 @@
       <c r="E21" s="8">
         <v>12</v>
       </c>
-      <c r="F21" s="26"/>
       <c r="G21" s="21">
         <f t="shared" si="8"/>
         <v>202</v>
       </c>
-      <c r="H21" s="23" t="str">
-        <f>D21</f>
-        <v>ASOKAM SA DE CV</v>
+      <c r="H21" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="I21" s="21">
         <f t="shared" si="9"/>
@@ -1521,7 +1532,6 @@
       <c r="E22" s="8">
         <v>6</v>
       </c>
-      <c r="F22" s="26"/>
       <c r="G22" s="21">
         <f t="shared" si="8"/>
         <v>208</v>
@@ -1560,7 +1570,6 @@
       <c r="E23" s="8">
         <v>6</v>
       </c>
-      <c r="F23" s="26"/>
       <c r="G23" s="21">
         <f t="shared" si="8"/>
         <v>210</v>
@@ -1598,13 +1607,12 @@
       <c r="E24" s="8">
         <v>3</v>
       </c>
-      <c r="F24" s="26"/>
       <c r="G24" s="21">
         <f t="shared" si="8"/>
         <v>217</v>
       </c>
       <c r="H24" s="23" t="str">
-        <f>D24</f>
+        <f t="shared" ref="H24:H33" si="10">D24</f>
         <v>COMVALSA</v>
       </c>
       <c r="I24" s="21">
@@ -1637,13 +1645,12 @@
       <c r="E25" s="8">
         <v>3</v>
       </c>
-      <c r="F25" s="26"/>
       <c r="G25" s="21">
         <f t="shared" si="8"/>
         <v>220</v>
       </c>
       <c r="H25" s="23" t="str">
-        <f>D25</f>
+        <f t="shared" si="10"/>
         <v>SWISS MEDICAL</v>
       </c>
       <c r="I25" s="21">
@@ -1674,13 +1681,12 @@
       <c r="E26" s="8">
         <v>2</v>
       </c>
-      <c r="F26" s="26"/>
       <c r="G26" s="21">
         <f t="shared" si="8"/>
         <v>224</v>
       </c>
       <c r="H26" s="23" t="str">
-        <f>D26</f>
+        <f t="shared" si="10"/>
         <v>SMNA</v>
       </c>
       <c r="I26" s="21">
@@ -1711,13 +1717,12 @@
       <c r="E27" s="8">
         <v>2</v>
       </c>
-      <c r="F27" s="26"/>
       <c r="G27" s="21">
         <f t="shared" si="8"/>
         <v>225</v>
       </c>
       <c r="H27" s="23" t="str">
-        <f>D27</f>
+        <f t="shared" si="10"/>
         <v>SOMAT / AMETD / SMAP</v>
       </c>
       <c r="I27" s="21">
@@ -1748,13 +1753,12 @@
       <c r="E28" s="8">
         <v>2</v>
       </c>
-      <c r="F28" s="26"/>
       <c r="G28" s="21">
         <f t="shared" si="8"/>
         <v>226</v>
       </c>
       <c r="H28" s="23" t="str">
-        <f>D28</f>
+        <f t="shared" si="10"/>
         <v>JOYERIA AZUL Y PLATA</v>
       </c>
       <c r="I28" s="21">
@@ -1787,13 +1791,12 @@
       <c r="E29" s="8">
         <v>12</v>
       </c>
-      <c r="F29" s="26"/>
       <c r="G29" s="21">
         <f t="shared" si="8"/>
         <v>302</v>
       </c>
       <c r="H29" s="23" t="str">
-        <f>D29</f>
+        <f t="shared" si="10"/>
         <v>LAERDAL</v>
       </c>
       <c r="I29" s="21">
@@ -1826,13 +1829,12 @@
       <c r="E30" s="8">
         <v>12</v>
       </c>
-      <c r="F30" s="26"/>
       <c r="G30" s="21">
         <f t="shared" si="8"/>
         <v>308</v>
       </c>
       <c r="H30" s="23" t="str">
-        <f>D30</f>
+        <f t="shared" si="10"/>
         <v>ALVARTIS PHARMA</v>
       </c>
       <c r="I30" s="21">
@@ -1865,13 +1867,12 @@
       <c r="E31" s="16">
         <v>6</v>
       </c>
-      <c r="F31" s="26"/>
       <c r="G31" s="21">
         <f t="shared" si="8"/>
         <v>314</v>
       </c>
       <c r="H31" s="23" t="str">
-        <f>D31</f>
+        <f t="shared" si="10"/>
         <v>MEDICAGAMA</v>
       </c>
       <c r="I31" s="21">
@@ -1904,13 +1905,12 @@
       <c r="E32" s="8">
         <v>3</v>
       </c>
-      <c r="F32" s="26"/>
       <c r="G32" s="21">
         <f t="shared" si="8"/>
         <v>316</v>
       </c>
       <c r="H32" s="23" t="str">
-        <f>D32</f>
+        <f t="shared" si="10"/>
         <v>SERTEC MEDICAL</v>
       </c>
       <c r="I32" s="21">
@@ -1943,13 +1943,12 @@
       <c r="E33" s="8">
         <v>3</v>
       </c>
-      <c r="F33" s="26"/>
       <c r="G33" s="21">
         <f t="shared" si="8"/>
         <v>320</v>
       </c>
       <c r="H33" s="23" t="str">
-        <f>D33</f>
+        <f t="shared" si="10"/>
         <v>LABORATORIOS SILANES</v>
       </c>
       <c r="I33" s="21">
@@ -1982,7 +1981,6 @@
       <c r="E34" s="16">
         <v>3</v>
       </c>
-      <c r="F34" s="26"/>
       <c r="G34" s="21">
         <f t="shared" si="8"/>
         <v>321</v>
@@ -2018,7 +2016,6 @@
       <c r="E35" s="16">
         <v>2</v>
       </c>
-      <c r="F35" s="26"/>
       <c r="G35" s="21">
         <f t="shared" si="8"/>
         <v>324</v>
@@ -2055,7 +2052,6 @@
       <c r="E36" s="16">
         <v>2</v>
       </c>
-      <c r="F36" s="26"/>
       <c r="G36" s="21">
         <f t="shared" si="8"/>
         <v>325</v>
@@ -2094,7 +2090,6 @@
       <c r="E37" s="8">
         <v>12</v>
       </c>
-      <c r="F37" s="26"/>
       <c r="G37" s="21">
         <f t="shared" si="8"/>
         <v>402</v>
@@ -2133,7 +2128,6 @@
       <c r="E38" s="8">
         <v>3</v>
       </c>
-      <c r="F38" s="26"/>
       <c r="G38" s="21">
         <f t="shared" si="8"/>
         <v>405</v>
@@ -2172,7 +2166,6 @@
       <c r="E39" s="8">
         <v>12</v>
       </c>
-      <c r="F39" s="26"/>
       <c r="G39" s="21">
         <f t="shared" si="8"/>
         <v>408</v>
@@ -2210,7 +2203,6 @@
       <c r="E40" s="8">
         <v>6</v>
       </c>
-      <c r="F40" s="26"/>
       <c r="G40" s="21">
         <f t="shared" si="8"/>
         <v>414</v>
@@ -2248,13 +2240,12 @@
       <c r="E41" s="8">
         <v>6</v>
       </c>
-      <c r="F41" s="26"/>
       <c r="G41" s="21">
         <f t="shared" si="8"/>
         <v>416</v>
       </c>
       <c r="H41" s="23" t="str">
-        <f>D41</f>
+        <f t="shared" ref="H41:H51" si="11">D41</f>
         <v>MENARINI</v>
       </c>
       <c r="I41" s="21">
@@ -2287,13 +2278,12 @@
       <c r="E42" s="8">
         <v>3</v>
       </c>
-      <c r="F42" s="26"/>
       <c r="G42" s="21">
         <f t="shared" si="8"/>
         <v>417</v>
       </c>
       <c r="H42" s="23" t="str">
-        <f>D42</f>
+        <f t="shared" si="11"/>
         <v>COMERCIALIZADORA LEO</v>
       </c>
       <c r="I42" s="21">
@@ -2326,13 +2316,12 @@
       <c r="E43" s="8">
         <v>3</v>
       </c>
-      <c r="F43" s="26"/>
       <c r="G43" s="21">
         <f t="shared" si="8"/>
         <v>420</v>
       </c>
       <c r="H43" s="23" t="str">
-        <f>D43</f>
+        <f t="shared" si="11"/>
         <v>MEDTRONIC</v>
       </c>
       <c r="I43" s="21">
@@ -2365,13 +2354,12 @@
       <c r="E44" s="8">
         <v>3</v>
       </c>
-      <c r="F44" s="26"/>
       <c r="G44" s="21">
         <f t="shared" si="8"/>
         <v>421</v>
       </c>
       <c r="H44" s="23" t="str">
-        <f>D44</f>
+        <f t="shared" si="11"/>
         <v>MEDICAL VIKINGS</v>
       </c>
       <c r="I44" s="21">
@@ -2404,13 +2392,12 @@
       <c r="E45" s="8">
         <v>3</v>
       </c>
-      <c r="F45" s="26"/>
       <c r="G45" s="21">
         <f t="shared" si="8"/>
         <v>424</v>
       </c>
       <c r="H45" s="23" t="str">
-        <f>D45</f>
+        <f t="shared" si="11"/>
         <v>DEFSA</v>
       </c>
       <c r="I45" s="21">
@@ -2441,13 +2428,12 @@
       <c r="E46" s="8">
         <v>2</v>
       </c>
-      <c r="F46" s="26"/>
       <c r="G46" s="21">
         <f t="shared" si="8"/>
         <v>425</v>
       </c>
       <c r="H46" s="23" t="str">
-        <f>D46</f>
+        <f t="shared" si="11"/>
         <v>ELSEVIER</v>
       </c>
       <c r="I46" s="21">
@@ -2480,13 +2466,12 @@
       <c r="E47" s="8">
         <v>3</v>
       </c>
-      <c r="F47" s="26"/>
       <c r="G47" s="21">
         <f t="shared" si="8"/>
         <v>506</v>
       </c>
       <c r="H47" s="23" t="str">
-        <f>D47</f>
+        <f t="shared" si="11"/>
         <v>FEDERACIÓN MEXICANA DE COLEGIOS DE ANESTESIOLOGÍA</v>
       </c>
       <c r="I47" s="21">
@@ -2519,13 +2504,12 @@
       <c r="E48" s="8">
         <v>6</v>
       </c>
-      <c r="F48" s="26"/>
       <c r="G48" s="21">
         <f t="shared" si="8"/>
         <v>508</v>
       </c>
       <c r="H48" s="23" t="str">
-        <f>D48</f>
+        <f t="shared" si="11"/>
         <v>SOLIDFARMA</v>
       </c>
       <c r="I48" s="21">
@@ -2558,13 +2542,12 @@
       <c r="E49" s="8">
         <v>3</v>
       </c>
-      <c r="F49" s="26"/>
       <c r="G49" s="21">
         <f t="shared" si="8"/>
         <v>521</v>
       </c>
       <c r="H49" s="23" t="str">
-        <f>D49</f>
+        <f t="shared" si="11"/>
         <v>EUROFARMA</v>
       </c>
       <c r="I49" s="21">
@@ -2597,13 +2580,12 @@
       <c r="E50" s="8">
         <v>6</v>
       </c>
-      <c r="F50" s="26"/>
       <c r="G50" s="21">
         <f t="shared" si="8"/>
         <v>522</v>
       </c>
       <c r="H50" s="23" t="str">
-        <f>D50</f>
+        <f t="shared" si="11"/>
         <v>AGEFINSA</v>
       </c>
       <c r="I50" s="21">
@@ -2636,13 +2618,12 @@
       <c r="E51" s="8">
         <v>3</v>
       </c>
-      <c r="F51" s="26"/>
       <c r="G51" s="21">
         <f t="shared" si="8"/>
         <v>525</v>
       </c>
       <c r="H51" s="23" t="str">
-        <f>D51</f>
+        <f t="shared" si="11"/>
         <v>GOBA</v>
       </c>
       <c r="I51" s="21">
@@ -2675,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C72EB62-7F22-463B-99C1-EE166EA95765}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3835,4 +3816,1217 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742F613E-6DBC-4A94-A790-CC9B5F23C1DE}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="57.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G2" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G3" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G4" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G5" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G6" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G7" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G8" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G9" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G10" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G11" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G12" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G13" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G14" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>202</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G15" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>208</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G16" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>210</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G17" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>217</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G18" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G19" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>224</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G20" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>225</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G21" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>226</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G22" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>302</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G23" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>308</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G24" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>314</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G25" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>316</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G26" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>320</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G27" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>321</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G28" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>324</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G29" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>325</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G30" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>402</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G31" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>405</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G32" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>408</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G33" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>414</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G34" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>416</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G35" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>417</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G36" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>420</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G37" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>421</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G38" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>424</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G39" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>425</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G40" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>506</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G41" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>508</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G42" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>521</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G43" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>522</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G44" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>525</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G45" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>999</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46">
+        <v>99</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="G46" s="27">
+        <v>45465.764097222222</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>